<commit_message>
adding data inputs and some outputs
</commit_message>
<xml_diff>
--- a/2021/01-klobouky/01-klobouky2021.xlsx
+++ b/2021/01-klobouky/01-klobouky2021.xlsx
@@ -391,7 +391,7 @@
     <t xml:space="preserve">Chytil Jan</t>
   </si>
   <si>
-    <t xml:space="preserve">Cyklo...</t>
+    <t xml:space="preserve">cyklotrenink.com</t>
   </si>
   <si>
     <t xml:space="preserve">Dittrich Jaroslav</t>
@@ -745,8 +745,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ177"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A94" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C130" activeCellId="0" sqref="C130"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A134" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D149" activeCellId="0" sqref="D149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.05" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>